<commit_message>
updates redd summary, up and up estimate metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/clear_redd_summary_metadata.xlsx
+++ b/data-raw/metadata/clear_redd_summary_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-clear-adult-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C231DADF-8D8A-44B2-BA1E-C1B19C95663B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B146E94C-6859-4890-BFF9-FE100FD9BE28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3230" yWindow="760" windowWidth="17190" windowHeight="13310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -121,13 +121,13 @@
     <t>149</t>
   </si>
   <si>
-    <t>2023</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>2024</t>
   </si>
 </sst>
 </file>
@@ -453,9 +453,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -562,7 +562,7 @@
         <v>29</v>
       </c>
       <c r="M2" s="16" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
@@ -607,7 +607,7 @@
       <c r="J3" s="15"/>
       <c r="K3" s="14"/>
       <c r="L3" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M3" s="16" t="s">
         <v>30</v>
@@ -655,7 +655,7 @@
       <c r="J4" s="15"/>
       <c r="K4" s="14"/>
       <c r="L4" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M4" s="16" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
updates redd summary metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/clear_redd_summary_metadata.xlsx
+++ b/data-raw/metadata/clear_redd_summary_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-clear-adult-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B146E94C-6859-4890-BFF9-FE100FD9BE28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A262B8-FCAD-4B29-9455-23D4AB58F84B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1990" yWindow="2140" windowWidth="19200" windowHeight="11180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -128,6 +128,18 @@
   </si>
   <si>
     <t>2024</t>
+  </si>
+  <si>
+    <t>Survey reach where survey was done</t>
+  </si>
+  <si>
+    <t>reach_numbers</t>
+  </si>
+  <si>
+    <t>ordinal</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
 </sst>
 </file>
@@ -453,9 +465,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -675,11 +687,21 @@
       <c r="Z4" s="7"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="4"/>
+      <c r="A5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>

</xml_diff>